<commit_message>
Criptografando senhas salvas no banco
</commit_message>
<xml_diff>
--- a/src/server/resources/startUpFiles/usersMock.xlsx
+++ b/src/server/resources/startUpFiles/usersMock.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://embraer-my.sharepoint.com/personal/roesney_embraer_com_br/Documents/Desktop/FSE/FATEC/eFOL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafs9\Desktop\Programação\Projeto Integrador\api-claradb\src\server\resources\startUpFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="8_{0C0D7B36-1635-402E-AB8B-C661BD15F166}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{B45AAEDA-8C56-47B7-A8FA-216032D26579}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED95AE5-8C9A-469A-8E4F-37A4B47CE5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="query" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
   <si>
     <t>Mercedes</t>
   </si>
@@ -239,6 +239,12 @@
   </si>
   <si>
     <t>maraujo</t>
+  </si>
+  <si>
+    <t>912857</t>
+  </si>
+  <si>
+    <t>501358</t>
   </si>
 </sst>
 </file>
@@ -728,50 +734,53 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bom" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Célula de Verificação" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Célula Vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Ênfase1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Ênfase2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Ênfase3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Ênfase4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Ênfase5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Ênfase6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Neutro" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Ruim" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -779,9 +788,6 @@
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -838,16 +844,16 @@
   <autoFilter ref="A1:D26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="Title" name="Username" queryTableFieldId="1" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{0F5F17B3-0CE3-4464-A2F1-CE8CD56D5756}" uniqueName="12" name="Login" queryTableFieldId="22" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{78EDE422-9E38-4E72-AD1C-62B7314CABF9}" uniqueName="11" name="Password" queryTableFieldId="21" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="Family" name="Equipment" queryTableFieldId="2" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{0F5F17B3-0CE3-4464-A2F1-CE8CD56D5756}" uniqueName="12" name="Login" queryTableFieldId="22" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{78EDE422-9E38-4E72-AD1C-62B7314CABF9}" uniqueName="11" name="Password" queryTableFieldId="21" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="Family" name="Equipment" queryTableFieldId="2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1146,7 +1152,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,8 +1183,8 @@
       <c r="B2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="1">
-        <v>501358</v>
+      <c r="C2" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>36</v>
@@ -1485,8 +1491,8 @@
       <c r="B24" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="1">
-        <v>912857</v>
+      <c r="C24" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>6</v>
@@ -1530,6 +1536,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MigrationWizIdVersion xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
+    <MigrationWizId xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
+    <MigrationWizIdPermissions xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D243F44452894F44B30B01D78AB550C6" ma:contentTypeVersion="17" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="ddf399ed8ada02634f296533fe838ba1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9418c341-2c26-482a-ba67-30e585bee0b1" xmlns:ns4="0091c14d-f26b-48ae-945a-e337a54cb016" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="963084035f90fff10d6e13b4c6188075" ns3:_="" ns4:_="">
     <xsd:import namespace="9418c341-2c26-482a-ba67-30e585bee0b1"/>
@@ -1776,26 +1801,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D03DEB8B-37EB-4B2F-B56C-F099DE211C01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="0091c14d-f26b-48ae-945a-e337a54cb016"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9418c341-2c26-482a-ba67-30e585bee0b1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MigrationWizIdVersion xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
-    <MigrationWizId xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
-    <MigrationWizIdPermissions xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23D559E3-0E90-4A20-9D4E-9F71DBFA59D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{086289FB-6338-4A25-B40D-540EB93B2F2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1812,29 +1843,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23D559E3-0E90-4A20-9D4E-9F71DBFA59D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D03DEB8B-37EB-4B2F-B56C-F099DE211C01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="0091c14d-f26b-48ae-945a-e337a54cb016"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9418c341-2c26-482a-ba67-30e585bee0b1"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Salvando ID do usuário e repassando para páginas
</commit_message>
<xml_diff>
--- a/src/server/resources/startUpFiles/usersMock.xlsx
+++ b/src/server/resources/startUpFiles/usersMock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafs9\Desktop\Programação\Projeto Integrador\api-claradb\src\server\resources\startUpFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED95AE5-8C9A-469A-8E4F-37A4B47CE5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A2645F-AEDD-4944-BD3D-1524E437A813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="query" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="query" localSheetId="0" hidden="1">query!$A$1:$D$26</definedName>
+    <definedName name="query" localSheetId="0" hidden="1">query!$A$1:$D$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
   <si>
     <t>Mercedes</t>
   </si>
@@ -245,6 +245,18 @@
   </si>
   <si>
     <t>501358</t>
+  </si>
+  <si>
+    <t>Rafael Furtado</t>
+  </si>
+  <si>
+    <t>syank</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>Porsche, BMW, Corvette, Mercedes, Mustang</t>
   </si>
 </sst>
 </file>
@@ -840,8 +852,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_query" displayName="Table_query" ref="A1:D26" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_query" displayName="Table_query" ref="A1:D27" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D27" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="Title" name="Username" queryTableFieldId="1" dataDxfId="3"/>
     <tableColumn id="12" xr3:uid="{0F5F17B3-0CE3-4464-A2F1-CE8CD56D5756}" uniqueName="12" name="Login" queryTableFieldId="22" dataDxfId="2"/>
@@ -1149,17 +1161,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1524,6 +1536,20 @@
       </c>
       <c r="D26" s="2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1536,25 +1562,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MigrationWizIdVersion xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
-    <MigrationWizId xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
-    <MigrationWizIdPermissions xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D243F44452894F44B30B01D78AB550C6" ma:contentTypeVersion="17" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="ddf399ed8ada02634f296533fe838ba1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9418c341-2c26-482a-ba67-30e585bee0b1" xmlns:ns4="0091c14d-f26b-48ae-945a-e337a54cb016" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="963084035f90fff10d6e13b4c6188075" ns3:_="" ns4:_="">
     <xsd:import namespace="9418c341-2c26-482a-ba67-30e585bee0b1"/>
@@ -1801,32 +1808,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D03DEB8B-37EB-4B2F-B56C-F099DE211C01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="0091c14d-f26b-48ae-945a-e337a54cb016"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9418c341-2c26-482a-ba67-30e585bee0b1"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23D559E3-0E90-4A20-9D4E-9F71DBFA59D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MigrationWizIdVersion xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
+    <MigrationWizId xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
+    <MigrationWizIdPermissions xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{086289FB-6338-4A25-B40D-540EB93B2F2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1843,4 +1844,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23D559E3-0E90-4A20-9D4E-9F71DBFA59D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D03DEB8B-37EB-4B2F-B56C-F099DE211C01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="0091c14d-f26b-48ae-945a-e337a54cb016"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9418c341-2c26-482a-ba67-30e585bee0b1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Pesquisando FOLs por status
</commit_message>
<xml_diff>
--- a/src/server/resources/startUpFiles/usersMock.xlsx
+++ b/src/server/resources/startUpFiles/usersMock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafs9\Desktop\Programação\Projeto Integrador\api-claradb\src\server\resources\startUpFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A2645F-AEDD-4944-BD3D-1524E437A813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D6D0C3-66CC-4CF6-81D3-967D3C6060D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="query" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="query" localSheetId="0" hidden="1">query!$A$1:$D$27</definedName>
+    <definedName name="query" localSheetId="0" hidden="1">query!$A$1:$D$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="75">
   <si>
     <t>Mercedes</t>
   </si>
@@ -257,6 +257,12 @@
   </si>
   <si>
     <t>Porsche, BMW, Corvette, Mercedes, Mustang</t>
+  </si>
+  <si>
+    <t>Anna Yukimi Yamada</t>
+  </si>
+  <si>
+    <t>iuquimi</t>
   </si>
 </sst>
 </file>
@@ -852,8 +858,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_query" displayName="Table_query" ref="A1:D27" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D27" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_query" displayName="Table_query" ref="A1:D28" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D28" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="Title" name="Username" queryTableFieldId="1" dataDxfId="3"/>
     <tableColumn id="12" xr3:uid="{0F5F17B3-0CE3-4464-A2F1-CE8CD56D5756}" uniqueName="12" name="Login" queryTableFieldId="22" dataDxfId="2"/>
@@ -1161,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1552,6 +1558,20 @@
         <v>72</v>
       </c>
     </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1562,6 +1582,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MigrationWizIdVersion xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
+    <MigrationWizId xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
+    <MigrationWizIdPermissions xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D243F44452894F44B30B01D78AB550C6" ma:contentTypeVersion="17" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="ddf399ed8ada02634f296533fe838ba1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9418c341-2c26-482a-ba67-30e585bee0b1" xmlns:ns4="0091c14d-f26b-48ae-945a-e337a54cb016" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="963084035f90fff10d6e13b4c6188075" ns3:_="" ns4:_="">
     <xsd:import namespace="9418c341-2c26-482a-ba67-30e585bee0b1"/>
@@ -1808,26 +1847,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D03DEB8B-37EB-4B2F-B56C-F099DE211C01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="0091c14d-f26b-48ae-945a-e337a54cb016"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9418c341-2c26-482a-ba67-30e585bee0b1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MigrationWizIdVersion xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
-    <MigrationWizId xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
-    <MigrationWizIdPermissions xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23D559E3-0E90-4A20-9D4E-9F71DBFA59D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{086289FB-6338-4A25-B40D-540EB93B2F2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1844,29 +1889,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23D559E3-0E90-4A20-9D4E-9F71DBFA59D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D03DEB8B-37EB-4B2F-B56C-F099DE211C01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="0091c14d-f26b-48ae-945a-e337a54cb016"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9418c341-2c26-482a-ba67-30e585bee0b1"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adding myself as an user :P
</commit_message>
<xml_diff>
--- a/src/server/resources/startUpFiles/usersMock.xlsx
+++ b/src/server/resources/startUpFiles/usersMock.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafs9\Desktop\Programação\Projeto Integrador\api-claradb\src\server\resources\startUpFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\port3\Desktop\api-claradb\src\server\resources\startUpFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D6D0C3-66CC-4CF6-81D3-967D3C6060D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8603BA24-4342-4C6C-988A-808B2141530B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="query" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="query" localSheetId="0" hidden="1">query!$A$1:$D$28</definedName>
+    <definedName name="query" localSheetId="0" hidden="1">query!$A$1:$D$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
   <si>
     <t>Mercedes</t>
   </si>
@@ -263,6 +263,15 @@
   </si>
   <si>
     <t>iuquimi</t>
+  </si>
+  <si>
+    <t>Bárbara Port</t>
+  </si>
+  <si>
+    <t>bport</t>
+  </si>
+  <si>
+    <t>Corvette, BMW</t>
   </si>
 </sst>
 </file>
@@ -858,8 +867,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_query" displayName="Table_query" ref="A1:D28" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D28" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_query" displayName="Table_query" ref="A1:D29" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="Title" name="Username" queryTableFieldId="1" dataDxfId="3"/>
     <tableColumn id="12" xr3:uid="{0F5F17B3-0CE3-4464-A2F1-CE8CD56D5756}" uniqueName="12" name="Login" queryTableFieldId="22" dataDxfId="2"/>
@@ -1167,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,15 +1569,29 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1582,25 +1605,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MigrationWizIdVersion xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
-    <MigrationWizId xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
-    <MigrationWizIdPermissions xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D243F44452894F44B30B01D78AB550C6" ma:contentTypeVersion="17" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="ddf399ed8ada02634f296533fe838ba1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9418c341-2c26-482a-ba67-30e585bee0b1" xmlns:ns4="0091c14d-f26b-48ae-945a-e337a54cb016" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="963084035f90fff10d6e13b4c6188075" ns3:_="" ns4:_="">
     <xsd:import namespace="9418c341-2c26-482a-ba67-30e585bee0b1"/>
@@ -1847,32 +1851,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D03DEB8B-37EB-4B2F-B56C-F099DE211C01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="0091c14d-f26b-48ae-945a-e337a54cb016"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9418c341-2c26-482a-ba67-30e585bee0b1"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23D559E3-0E90-4A20-9D4E-9F71DBFA59D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MigrationWizIdVersion xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
+    <MigrationWizId xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
+    <MigrationWizIdPermissions xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{086289FB-6338-4A25-B40D-540EB93B2F2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1889,4 +1887,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23D559E3-0E90-4A20-9D4E-9F71DBFA59D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D03DEB8B-37EB-4B2F-B56C-F099DE211C01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="0091c14d-f26b-48ae-945a-e337a54cb016"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9418c341-2c26-482a-ba67-30e585bee0b1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adding a mustang to myself
</commit_message>
<xml_diff>
--- a/src/server/resources/startUpFiles/usersMock.xlsx
+++ b/src/server/resources/startUpFiles/usersMock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\port3\Desktop\api-claradb\src\server\resources\startUpFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8603BA24-4342-4C6C-988A-808B2141530B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FCEF5D-FC2C-48F6-A4D5-32E5952B6E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -271,7 +271,7 @@
     <t>bport</t>
   </si>
   <si>
-    <t>Corvette, BMW</t>
+    <t>Corvette, BMW, Mustang</t>
   </si>
 </sst>
 </file>
@@ -1179,7 +1179,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1605,6 +1605,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MigrationWizIdVersion xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
+    <MigrationWizId xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
+    <MigrationWizIdPermissions xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D243F44452894F44B30B01D78AB550C6" ma:contentTypeVersion="17" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="ddf399ed8ada02634f296533fe838ba1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9418c341-2c26-482a-ba67-30e585bee0b1" xmlns:ns4="0091c14d-f26b-48ae-945a-e337a54cb016" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="963084035f90fff10d6e13b4c6188075" ns3:_="" ns4:_="">
     <xsd:import namespace="9418c341-2c26-482a-ba67-30e585bee0b1"/>
@@ -1851,26 +1870,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D03DEB8B-37EB-4B2F-B56C-F099DE211C01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="0091c14d-f26b-48ae-945a-e337a54cb016"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9418c341-2c26-482a-ba67-30e585bee0b1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MigrationWizIdVersion xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
-    <MigrationWizId xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
-    <MigrationWizIdPermissions xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23D559E3-0E90-4A20-9D4E-9F71DBFA59D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{086289FB-6338-4A25-B40D-540EB93B2F2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1887,29 +1912,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23D559E3-0E90-4A20-9D4E-9F71DBFA59D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D03DEB8B-37EB-4B2F-B56C-F099DE211C01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="0091c14d-f26b-48ae-945a-e337a54cb016"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9418c341-2c26-482a-ba67-30e585bee0b1"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Criando observador de arquivos
</commit_message>
<xml_diff>
--- a/src/server/resources/startUpFiles/usersMock.xlsx
+++ b/src/server/resources/startUpFiles/usersMock.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\port3\Desktop\api-claradb\src\server\resources\startUpFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafs9\Desktop\Programacao\ProjetoIntegrador\api-claradb\src\server\resources\startUpFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FCEF5D-FC2C-48F6-A4D5-32E5952B6E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0AEF8B-3516-415C-BF37-451BB1E85B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4710" yWindow="1680" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="query" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="77">
   <si>
     <t>Mercedes</t>
   </si>
@@ -254,9 +254,6 @@
   </si>
   <si>
     <t>123456</t>
-  </si>
-  <si>
-    <t>Porsche, BMW, Corvette, Mercedes, Mustang</t>
   </si>
   <si>
     <t>Anna Yukimi Yamada</t>
@@ -1178,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,29 +1561,29 @@
         <v>71</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>71</v>
@@ -1605,25 +1602,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MigrationWizIdVersion xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
-    <MigrationWizId xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
-    <MigrationWizIdPermissions xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D243F44452894F44B30B01D78AB550C6" ma:contentTypeVersion="17" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="ddf399ed8ada02634f296533fe838ba1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9418c341-2c26-482a-ba67-30e585bee0b1" xmlns:ns4="0091c14d-f26b-48ae-945a-e337a54cb016" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="963084035f90fff10d6e13b4c6188075" ns3:_="" ns4:_="">
     <xsd:import namespace="9418c341-2c26-482a-ba67-30e585bee0b1"/>
@@ -1870,32 +1848,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D03DEB8B-37EB-4B2F-B56C-F099DE211C01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="0091c14d-f26b-48ae-945a-e337a54cb016"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9418c341-2c26-482a-ba67-30e585bee0b1"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23D559E3-0E90-4A20-9D4E-9F71DBFA59D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MigrationWizIdVersion xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
+    <MigrationWizId xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
+    <MigrationWizIdPermissions xmlns="0091c14d-f26b-48ae-945a-e337a54cb016" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{086289FB-6338-4A25-B40D-540EB93B2F2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1912,4 +1884,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23D559E3-0E90-4A20-9D4E-9F71DBFA59D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D03DEB8B-37EB-4B2F-B56C-F099DE211C01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="0091c14d-f26b-48ae-945a-e337a54cb016"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9418c341-2c26-482a-ba67-30e585bee0b1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>